<commit_message>
random number tested till 5000 numbers and img added
</commit_message>
<xml_diff>
--- a/katatsubaVSgradeschool.xlsx
+++ b/katatsubaVSgradeschool.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Digits</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Num/Sec</t>
+  </si>
+  <si>
+    <t>Num/sec</t>
   </si>
 </sst>
 </file>
@@ -111,8 +114,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -159,7 +170,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -181,6 +192,10 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -202,6 +217,10 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,11 +428,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2027872008"/>
-        <c:axId val="2119061240"/>
+        <c:axId val="2115728552"/>
+        <c:axId val="2115718040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2027872008"/>
+        <c:axId val="2115728552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,7 +460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119061240"/>
+        <c:crossAx val="2115718040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -449,7 +468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119061240"/>
+        <c:axId val="2115718040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,7 +496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2027872008"/>
+        <c:crossAx val="2115728552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3521,9 +3540,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AQ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -3533,7 +3552,7 @@
     <col min="27" max="27" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:43">
       <c r="A1">
         <v>501</v>
       </c>
@@ -3555,8 +3574,20 @@
       <c r="Y1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="2" spans="1:27">
+      <c r="AC1">
+        <v>3500</v>
+      </c>
+      <c r="AG1">
+        <v>4000</v>
+      </c>
+      <c r="AK1">
+        <v>4500</v>
+      </c>
+      <c r="AO1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="G2" t="s">
         <v>10</v>
       </c>
@@ -3569,8 +3600,23 @@
       <c r="S2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:27">
+      <c r="W2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
       <c r="E4">
         <v>117</v>
       </c>
@@ -3637,8 +3683,52 @@
         <f>$Y$1/Z4</f>
         <v>4559.2705167173253</v>
       </c>
-    </row>
-    <row r="5" spans="1:27">
+      <c r="AC4">
+        <v>748</v>
+      </c>
+      <c r="AD4">
+        <f>AC4/1000</f>
+        <v>0.748</v>
+      </c>
+      <c r="AE4">
+        <f>$AC$1/AD4</f>
+        <v>4679.1443850267378</v>
+      </c>
+      <c r="AG4">
+        <v>867</v>
+      </c>
+      <c r="AH4">
+        <f>AG4/1000</f>
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="AI4">
+        <f>$AG$1/AH4</f>
+        <v>4613.6101499423303</v>
+      </c>
+      <c r="AK4">
+        <v>976</v>
+      </c>
+      <c r="AL4">
+        <f>AK4/1000</f>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AM4">
+        <f>$AK$1/AL4</f>
+        <v>4610.6557377049185</v>
+      </c>
+      <c r="AO4">
+        <v>1098</v>
+      </c>
+      <c r="AP4">
+        <f>AO4/1000</f>
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="AQ4">
+        <f>$AO$1/AP4</f>
+        <v>4553.7340619307824</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43">
       <c r="E5">
         <v>110</v>
       </c>
@@ -3705,8 +3795,52 @@
         <f t="shared" ref="AA5:AA33" si="11">$Y$1/Z5</f>
         <v>4665.6298600311038</v>
       </c>
-    </row>
-    <row r="6" spans="1:27">
+      <c r="AC5">
+        <v>749</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" ref="AD5:AD33" si="12">AC5/1000</f>
+        <v>0.749</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" ref="AE5:AE33" si="13">$AC$1/AD5</f>
+        <v>4672.8971962616824</v>
+      </c>
+      <c r="AG5">
+        <v>866</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" ref="AH5:AH33" si="14">AG5/1000</f>
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" ref="AI5:AI33" si="15">$AG$1/AH5</f>
+        <v>4618.9376443418014</v>
+      </c>
+      <c r="AK5">
+        <v>1060</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" ref="AL5:AL33" si="16">AK5/1000</f>
+        <v>1.06</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" ref="AM5:AM33" si="17">$AK$1/AL5</f>
+        <v>4245.2830188679245</v>
+      </c>
+      <c r="AO5">
+        <v>1180</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" ref="AP5:AP33" si="18">AO5/1000</f>
+        <v>1.18</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" ref="AQ5:AQ33" si="19">$AO$1/AP5</f>
+        <v>4237.2881355932204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
       <c r="E6">
         <v>110</v>
       </c>
@@ -3773,8 +3907,52 @@
         <f t="shared" si="11"/>
         <v>4615.3846153846152</v>
       </c>
-    </row>
-    <row r="7" spans="1:27">
+      <c r="AC6">
+        <v>743</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="12"/>
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="13"/>
+        <v>4710.6325706594889</v>
+      </c>
+      <c r="AG6">
+        <v>862</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="14"/>
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="15"/>
+        <v>4640.3712296983758</v>
+      </c>
+      <c r="AK6">
+        <v>991</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" si="16"/>
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="17"/>
+        <v>4540.8678102926333</v>
+      </c>
+      <c r="AO6">
+        <v>1141</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" si="18"/>
+        <v>1.141</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" si="19"/>
+        <v>4382.1209465381244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
       <c r="E7">
         <v>117</v>
       </c>
@@ -3841,8 +4019,52 @@
         <f t="shared" si="11"/>
         <v>4573.1707317073169</v>
       </c>
-    </row>
-    <row r="8" spans="1:27">
+      <c r="AC7">
+        <v>745</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="12"/>
+        <v>0.745</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="13"/>
+        <v>4697.9865771812083</v>
+      </c>
+      <c r="AG7">
+        <v>864</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="14"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="15"/>
+        <v>4629.6296296296296</v>
+      </c>
+      <c r="AK7">
+        <v>979</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="16"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="17"/>
+        <v>4596.5270684371808</v>
+      </c>
+      <c r="AO7">
+        <v>1091</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="18"/>
+        <v>1.091</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="19"/>
+        <v>4582.9514207149405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
       <c r="E8">
         <v>110</v>
       </c>
@@ -3909,8 +4131,52 @@
         <f t="shared" si="11"/>
         <v>4643.9628482972139</v>
       </c>
-    </row>
-    <row r="9" spans="1:27">
+      <c r="AC8">
+        <v>747</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="12"/>
+        <v>0.747</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="13"/>
+        <v>4685.4082998661315</v>
+      </c>
+      <c r="AG8">
+        <v>863</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="14"/>
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="15"/>
+        <v>4634.9942062572418</v>
+      </c>
+      <c r="AK8">
+        <v>985</v>
+      </c>
+      <c r="AL8">
+        <f t="shared" si="16"/>
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="17"/>
+        <v>4568.5279187817259</v>
+      </c>
+      <c r="AO8">
+        <v>1081</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" si="18"/>
+        <v>1.081</v>
+      </c>
+      <c r="AQ8">
+        <f t="shared" si="19"/>
+        <v>4625.3469010175768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="E9">
         <v>108</v>
       </c>
@@ -3977,8 +4243,52 @@
         <f t="shared" si="11"/>
         <v>4497.7511244377811</v>
       </c>
-    </row>
-    <row r="10" spans="1:27">
+      <c r="AC9">
+        <v>752</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="12"/>
+        <v>0.752</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="13"/>
+        <v>4654.255319148936</v>
+      </c>
+      <c r="AG9">
+        <v>860</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="14"/>
+        <v>0.86</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="15"/>
+        <v>4651.1627906976746</v>
+      </c>
+      <c r="AK9">
+        <v>972</v>
+      </c>
+      <c r="AL9">
+        <f t="shared" si="16"/>
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="17"/>
+        <v>4629.6296296296296</v>
+      </c>
+      <c r="AO9">
+        <v>1098</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="18"/>
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="AQ9">
+        <f t="shared" si="19"/>
+        <v>4553.7340619307824</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43">
       <c r="E10">
         <v>108</v>
       </c>
@@ -4045,8 +4355,52 @@
         <f t="shared" si="11"/>
         <v>4658.3850931677016</v>
       </c>
-    </row>
-    <row r="11" spans="1:27">
+      <c r="AC10">
+        <v>747</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="12"/>
+        <v>0.747</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="13"/>
+        <v>4685.4082998661315</v>
+      </c>
+      <c r="AG10">
+        <v>855</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="14"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="15"/>
+        <v>4678.3625730994154</v>
+      </c>
+      <c r="AK10">
+        <v>967</v>
+      </c>
+      <c r="AL10">
+        <f t="shared" si="16"/>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="17"/>
+        <v>4653.5677352637022</v>
+      </c>
+      <c r="AO10">
+        <v>1075</v>
+      </c>
+      <c r="AP10">
+        <f t="shared" si="18"/>
+        <v>1.075</v>
+      </c>
+      <c r="AQ10">
+        <f t="shared" si="19"/>
+        <v>4651.1627906976746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="E11">
         <v>120</v>
       </c>
@@ -4113,8 +4467,52 @@
         <f t="shared" si="11"/>
         <v>4545.454545454545</v>
       </c>
-    </row>
-    <row r="12" spans="1:27">
+      <c r="AC11">
+        <v>744</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="12"/>
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="13"/>
+        <v>4704.3010752688169</v>
+      </c>
+      <c r="AG11">
+        <v>862</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="14"/>
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="15"/>
+        <v>4640.3712296983758</v>
+      </c>
+      <c r="AK11">
+        <v>975</v>
+      </c>
+      <c r="AL11">
+        <f t="shared" si="16"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="17"/>
+        <v>4615.3846153846152</v>
+      </c>
+      <c r="AO11">
+        <v>1075</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" si="18"/>
+        <v>1.075</v>
+      </c>
+      <c r="AQ11">
+        <f t="shared" si="19"/>
+        <v>4651.1627906976746</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="E12">
         <v>115</v>
       </c>
@@ -4181,8 +4579,52 @@
         <f t="shared" si="11"/>
         <v>4622.4961479198764</v>
       </c>
-    </row>
-    <row r="13" spans="1:27">
+      <c r="AC12">
+        <v>747</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="12"/>
+        <v>0.747</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="13"/>
+        <v>4685.4082998661315</v>
+      </c>
+      <c r="AG12">
+        <v>866</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="14"/>
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="15"/>
+        <v>4618.9376443418014</v>
+      </c>
+      <c r="AK12">
+        <v>980</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="16"/>
+        <v>0.98</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="17"/>
+        <v>4591.8367346938776</v>
+      </c>
+      <c r="AO12">
+        <v>1085</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="18"/>
+        <v>1.085</v>
+      </c>
+      <c r="AQ12">
+        <f t="shared" si="19"/>
+        <v>4608.294930875576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="E13">
         <v>112</v>
       </c>
@@ -4249,8 +4691,52 @@
         <f t="shared" si="11"/>
         <v>4629.6296296296296</v>
       </c>
-    </row>
-    <row r="14" spans="1:27">
+      <c r="AC13">
+        <v>740</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="12"/>
+        <v>0.74</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="13"/>
+        <v>4729.72972972973</v>
+      </c>
+      <c r="AG13">
+        <v>866</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="14"/>
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="15"/>
+        <v>4618.9376443418014</v>
+      </c>
+      <c r="AK13">
+        <v>1007</v>
+      </c>
+      <c r="AL13">
+        <f t="shared" si="16"/>
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="AM13">
+        <f t="shared" si="17"/>
+        <v>4468.7189672293944</v>
+      </c>
+      <c r="AO13">
+        <v>1090</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="18"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AQ13">
+        <f t="shared" si="19"/>
+        <v>4587.1559633027518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="E14">
         <v>109</v>
       </c>
@@ -4317,8 +4803,52 @@
         <f t="shared" si="11"/>
         <v>4651.1627906976746</v>
       </c>
-    </row>
-    <row r="15" spans="1:27">
+      <c r="AC14">
+        <v>745</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="12"/>
+        <v>0.745</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="13"/>
+        <v>4697.9865771812083</v>
+      </c>
+      <c r="AG14">
+        <v>867</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="14"/>
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="15"/>
+        <v>4613.6101499423303</v>
+      </c>
+      <c r="AK14">
+        <v>1002</v>
+      </c>
+      <c r="AL14">
+        <f t="shared" si="16"/>
+        <v>1.002</v>
+      </c>
+      <c r="AM14">
+        <f t="shared" si="17"/>
+        <v>4491.0179640718561</v>
+      </c>
+      <c r="AO14">
+        <v>1088</v>
+      </c>
+      <c r="AP14">
+        <f t="shared" si="18"/>
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="AQ14">
+        <f t="shared" si="19"/>
+        <v>4595.5882352941171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43">
       <c r="E15">
         <v>114</v>
       </c>
@@ -4385,8 +4915,52 @@
         <f t="shared" si="11"/>
         <v>4594.1807044410416</v>
       </c>
-    </row>
-    <row r="16" spans="1:27">
+      <c r="AC15">
+        <v>749</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="12"/>
+        <v>0.749</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="13"/>
+        <v>4672.8971962616824</v>
+      </c>
+      <c r="AG15">
+        <v>876</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="14"/>
+        <v>0.876</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="15"/>
+        <v>4566.2100456621001</v>
+      </c>
+      <c r="AK15">
+        <v>977</v>
+      </c>
+      <c r="AL15">
+        <f t="shared" si="16"/>
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="17"/>
+        <v>4605.9365404298878</v>
+      </c>
+      <c r="AO15">
+        <v>1100</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="18"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="19"/>
+        <v>4545.454545454545</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43">
       <c r="E16">
         <v>111</v>
       </c>
@@ -4453,8 +5027,52 @@
         <f t="shared" si="11"/>
         <v>4643.9628482972139</v>
       </c>
-    </row>
-    <row r="17" spans="5:27">
+      <c r="AC16">
+        <v>742</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="12"/>
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="13"/>
+        <v>4716.9811320754716</v>
+      </c>
+      <c r="AG16">
+        <v>868</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="14"/>
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="AI16">
+        <f t="shared" si="15"/>
+        <v>4608.294930875576</v>
+      </c>
+      <c r="AK16">
+        <v>990</v>
+      </c>
+      <c r="AL16">
+        <f t="shared" si="16"/>
+        <v>0.99</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" si="17"/>
+        <v>4545.454545454545</v>
+      </c>
+      <c r="AO16">
+        <v>1121</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="18"/>
+        <v>1.121</v>
+      </c>
+      <c r="AQ16">
+        <f t="shared" si="19"/>
+        <v>4460.3033006244423</v>
+      </c>
+    </row>
+    <row r="17" spans="5:43">
       <c r="E17">
         <v>107</v>
       </c>
@@ -4521,8 +5139,52 @@
         <f t="shared" si="11"/>
         <v>4545.454545454545</v>
       </c>
-    </row>
-    <row r="18" spans="5:27">
+      <c r="AC17">
+        <v>765</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="12"/>
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="13"/>
+        <v>4575.16339869281</v>
+      </c>
+      <c r="AG17">
+        <v>859</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="14"/>
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="AI17">
+        <f t="shared" si="15"/>
+        <v>4656.5774155995341</v>
+      </c>
+      <c r="AK17">
+        <v>975</v>
+      </c>
+      <c r="AL17">
+        <f t="shared" si="16"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="17"/>
+        <v>4615.3846153846152</v>
+      </c>
+      <c r="AO17">
+        <v>1086</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="18"/>
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="AQ17">
+        <f t="shared" si="19"/>
+        <v>4604.0515653775319</v>
+      </c>
+    </row>
+    <row r="18" spans="5:43">
       <c r="E18">
         <v>113</v>
       </c>
@@ -4589,8 +5251,52 @@
         <f t="shared" si="11"/>
         <v>4538.5779122541599</v>
       </c>
-    </row>
-    <row r="19" spans="5:27">
+      <c r="AC18">
+        <v>749</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="12"/>
+        <v>0.749</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="13"/>
+        <v>4672.8971962616824</v>
+      </c>
+      <c r="AG18">
+        <v>855</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="14"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="15"/>
+        <v>4678.3625730994154</v>
+      </c>
+      <c r="AK18">
+        <v>967</v>
+      </c>
+      <c r="AL18">
+        <f t="shared" si="16"/>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="17"/>
+        <v>4653.5677352637022</v>
+      </c>
+      <c r="AO18">
+        <v>1091</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" si="18"/>
+        <v>1.091</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" si="19"/>
+        <v>4582.9514207149405</v>
+      </c>
+    </row>
+    <row r="19" spans="5:43">
       <c r="E19">
         <v>107</v>
       </c>
@@ -4657,8 +5363,52 @@
         <f t="shared" si="11"/>
         <v>4608.294930875576</v>
       </c>
-    </row>
-    <row r="20" spans="5:27">
+      <c r="AC19">
+        <v>783</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="12"/>
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="13"/>
+        <v>4469.987228607918</v>
+      </c>
+      <c r="AG19">
+        <v>865</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="14"/>
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="AI19">
+        <f t="shared" si="15"/>
+        <v>4624.277456647399</v>
+      </c>
+      <c r="AK19">
+        <v>986</v>
+      </c>
+      <c r="AL19">
+        <f t="shared" si="16"/>
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="17"/>
+        <v>4563.8945233265722</v>
+      </c>
+      <c r="AO19">
+        <v>1085</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" si="18"/>
+        <v>1.085</v>
+      </c>
+      <c r="AQ19">
+        <f t="shared" si="19"/>
+        <v>4608.294930875576</v>
+      </c>
+    </row>
+    <row r="20" spans="5:43">
       <c r="E20">
         <v>109</v>
       </c>
@@ -4725,8 +5475,52 @@
         <f t="shared" si="11"/>
         <v>4658.3850931677016</v>
       </c>
-    </row>
-    <row r="21" spans="5:27">
+      <c r="AC20">
+        <v>772</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="12"/>
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="13"/>
+        <v>4533.6787564766837</v>
+      </c>
+      <c r="AG20">
+        <v>859</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="14"/>
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="15"/>
+        <v>4656.5774155995341</v>
+      </c>
+      <c r="AK20">
+        <v>987</v>
+      </c>
+      <c r="AL20">
+        <f t="shared" si="16"/>
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="17"/>
+        <v>4559.2705167173253</v>
+      </c>
+      <c r="AO20">
+        <v>1077</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" si="18"/>
+        <v>1.077</v>
+      </c>
+      <c r="AQ20">
+        <f t="shared" si="19"/>
+        <v>4642.5255338904362</v>
+      </c>
+    </row>
+    <row r="21" spans="5:43">
       <c r="E21">
         <v>107</v>
       </c>
@@ -4793,8 +5587,52 @@
         <f t="shared" si="11"/>
         <v>4552.3520485584213</v>
       </c>
-    </row>
-    <row r="22" spans="5:27">
+      <c r="AC21">
+        <v>768</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="12"/>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="13"/>
+        <v>4557.291666666667</v>
+      </c>
+      <c r="AG21">
+        <v>874</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="14"/>
+        <v>0.874</v>
+      </c>
+      <c r="AI21">
+        <f t="shared" si="15"/>
+        <v>4576.6590389016019</v>
+      </c>
+      <c r="AK21">
+        <v>986</v>
+      </c>
+      <c r="AL21">
+        <f t="shared" si="16"/>
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="17"/>
+        <v>4563.8945233265722</v>
+      </c>
+      <c r="AO21">
+        <v>1082</v>
+      </c>
+      <c r="AP21">
+        <f t="shared" si="18"/>
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="AQ21">
+        <f t="shared" si="19"/>
+        <v>4621.0720887245834</v>
+      </c>
+    </row>
+    <row r="22" spans="5:43">
       <c r="E22">
         <v>107</v>
       </c>
@@ -4861,8 +5699,52 @@
         <f t="shared" si="11"/>
         <v>4665.6298600311038</v>
       </c>
-    </row>
-    <row r="23" spans="5:27">
+      <c r="AC22">
+        <v>759</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="12"/>
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="AE22">
+        <f t="shared" si="13"/>
+        <v>4611.33069828722</v>
+      </c>
+      <c r="AG22">
+        <v>875</v>
+      </c>
+      <c r="AH22">
+        <f t="shared" si="14"/>
+        <v>0.875</v>
+      </c>
+      <c r="AI22">
+        <f t="shared" si="15"/>
+        <v>4571.4285714285716</v>
+      </c>
+      <c r="AK22">
+        <v>971</v>
+      </c>
+      <c r="AL22">
+        <f t="shared" si="16"/>
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="AM22">
+        <f t="shared" si="17"/>
+        <v>4634.3975283213185</v>
+      </c>
+      <c r="AO22">
+        <v>1088</v>
+      </c>
+      <c r="AP22">
+        <f t="shared" si="18"/>
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="AQ22">
+        <f t="shared" si="19"/>
+        <v>4595.5882352941171</v>
+      </c>
+    </row>
+    <row r="23" spans="5:43">
       <c r="E23">
         <v>107</v>
       </c>
@@ -4929,8 +5811,52 @@
         <f t="shared" si="11"/>
         <v>4622.4961479198764</v>
       </c>
-    </row>
-    <row r="24" spans="5:27">
+      <c r="AC23">
+        <v>775</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="12"/>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="13"/>
+        <v>4516.1290322580644</v>
+      </c>
+      <c r="AG23">
+        <v>874</v>
+      </c>
+      <c r="AH23">
+        <f t="shared" si="14"/>
+        <v>0.874</v>
+      </c>
+      <c r="AI23">
+        <f t="shared" si="15"/>
+        <v>4576.6590389016019</v>
+      </c>
+      <c r="AK23">
+        <v>978</v>
+      </c>
+      <c r="AL23">
+        <f t="shared" si="16"/>
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="17"/>
+        <v>4601.2269938650306</v>
+      </c>
+      <c r="AO23">
+        <v>1090</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="18"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="19"/>
+        <v>4587.1559633027518</v>
+      </c>
+    </row>
+    <row r="24" spans="5:43">
       <c r="E24">
         <v>111</v>
       </c>
@@ -4997,8 +5923,52 @@
         <f t="shared" si="11"/>
         <v>4658.3850931677016</v>
       </c>
-    </row>
-    <row r="25" spans="5:27">
+      <c r="AC24">
+        <v>781</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="12"/>
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="13"/>
+        <v>4481.4340588988471</v>
+      </c>
+      <c r="AG24">
+        <v>855</v>
+      </c>
+      <c r="AH24">
+        <f t="shared" si="14"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="AI24">
+        <f t="shared" si="15"/>
+        <v>4678.3625730994154</v>
+      </c>
+      <c r="AK24">
+        <v>974</v>
+      </c>
+      <c r="AL24">
+        <f t="shared" si="16"/>
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="AM24">
+        <f t="shared" si="17"/>
+        <v>4620.1232032854214</v>
+      </c>
+      <c r="AO24">
+        <v>1085</v>
+      </c>
+      <c r="AP24">
+        <f t="shared" si="18"/>
+        <v>1.085</v>
+      </c>
+      <c r="AQ24">
+        <f t="shared" si="19"/>
+        <v>4608.294930875576</v>
+      </c>
+    </row>
+    <row r="25" spans="5:43">
       <c r="E25">
         <v>108</v>
       </c>
@@ -5065,8 +6035,52 @@
         <f t="shared" si="11"/>
         <v>4608.294930875576</v>
       </c>
-    </row>
-    <row r="26" spans="5:27">
+      <c r="AC25">
+        <v>818</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="12"/>
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="13"/>
+        <v>4278.7286063569682</v>
+      </c>
+      <c r="AG25">
+        <v>854</v>
+      </c>
+      <c r="AH25">
+        <f t="shared" si="14"/>
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="AI25">
+        <f t="shared" si="15"/>
+        <v>4683.8407494145204</v>
+      </c>
+      <c r="AK25">
+        <v>963</v>
+      </c>
+      <c r="AL25">
+        <f t="shared" si="16"/>
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="AM25">
+        <f t="shared" si="17"/>
+        <v>4672.8971962616824</v>
+      </c>
+      <c r="AO25">
+        <v>1090</v>
+      </c>
+      <c r="AP25">
+        <f t="shared" si="18"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AQ25">
+        <f t="shared" si="19"/>
+        <v>4587.1559633027518</v>
+      </c>
+    </row>
+    <row r="26" spans="5:43">
       <c r="E26">
         <v>107</v>
       </c>
@@ -5133,8 +6147,52 @@
         <f t="shared" si="11"/>
         <v>4594.1807044410416</v>
       </c>
-    </row>
-    <row r="27" spans="5:27">
+      <c r="AC26">
+        <v>772</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="12"/>
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="13"/>
+        <v>4533.6787564766837</v>
+      </c>
+      <c r="AG26">
+        <v>870</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="14"/>
+        <v>0.87</v>
+      </c>
+      <c r="AI26">
+        <f t="shared" si="15"/>
+        <v>4597.7011494252874</v>
+      </c>
+      <c r="AK26">
+        <v>985</v>
+      </c>
+      <c r="AL26">
+        <f t="shared" si="16"/>
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="17"/>
+        <v>4568.5279187817259</v>
+      </c>
+      <c r="AO26">
+        <v>1077</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="18"/>
+        <v>1.077</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="19"/>
+        <v>4642.5255338904362</v>
+      </c>
+    </row>
+    <row r="27" spans="5:43">
       <c r="E27">
         <v>115</v>
       </c>
@@ -5201,8 +6259,52 @@
         <f t="shared" si="11"/>
         <v>4545.454545454545</v>
       </c>
-    </row>
-    <row r="28" spans="5:27">
+      <c r="AC27">
+        <v>764</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="12"/>
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" si="13"/>
+        <v>4581.1518324607332</v>
+      </c>
+      <c r="AG27">
+        <v>863</v>
+      </c>
+      <c r="AH27">
+        <f t="shared" si="14"/>
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="AI27">
+        <f t="shared" si="15"/>
+        <v>4634.9942062572418</v>
+      </c>
+      <c r="AK27">
+        <v>979</v>
+      </c>
+      <c r="AL27">
+        <f t="shared" si="16"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AM27">
+        <f t="shared" si="17"/>
+        <v>4596.5270684371808</v>
+      </c>
+      <c r="AO27">
+        <v>1092</v>
+      </c>
+      <c r="AP27">
+        <f t="shared" si="18"/>
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="AQ27">
+        <f t="shared" si="19"/>
+        <v>4578.7545787545787</v>
+      </c>
+    </row>
+    <row r="28" spans="5:43">
       <c r="E28">
         <v>111</v>
       </c>
@@ -5269,8 +6371,52 @@
         <f t="shared" si="11"/>
         <v>4504.5045045045044</v>
       </c>
-    </row>
-    <row r="29" spans="5:27">
+      <c r="AC28">
+        <v>762</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="12"/>
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="13"/>
+        <v>4593.1758530183724</v>
+      </c>
+      <c r="AG28">
+        <v>857</v>
+      </c>
+      <c r="AH28">
+        <f t="shared" si="14"/>
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="AI28">
+        <f t="shared" si="15"/>
+        <v>4667.4445740956826</v>
+      </c>
+      <c r="AK28">
+        <v>969</v>
+      </c>
+      <c r="AL28">
+        <f t="shared" si="16"/>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="AM28">
+        <f t="shared" si="17"/>
+        <v>4643.9628482972139</v>
+      </c>
+      <c r="AO28">
+        <v>1091</v>
+      </c>
+      <c r="AP28">
+        <f t="shared" si="18"/>
+        <v>1.091</v>
+      </c>
+      <c r="AQ28">
+        <f t="shared" si="19"/>
+        <v>4582.9514207149405</v>
+      </c>
+    </row>
+    <row r="29" spans="5:43">
       <c r="E29">
         <v>110</v>
       </c>
@@ -5337,8 +6483,52 @@
         <f t="shared" si="11"/>
         <v>4531.7220543806643</v>
       </c>
-    </row>
-    <row r="30" spans="5:27">
+      <c r="AC29">
+        <v>799</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="12"/>
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="13"/>
+        <v>4380.4755944931158</v>
+      </c>
+      <c r="AG29">
+        <v>857</v>
+      </c>
+      <c r="AH29">
+        <f t="shared" si="14"/>
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="AI29">
+        <f t="shared" si="15"/>
+        <v>4667.4445740956826</v>
+      </c>
+      <c r="AK29">
+        <v>975</v>
+      </c>
+      <c r="AL29">
+        <f t="shared" si="16"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AM29">
+        <f t="shared" si="17"/>
+        <v>4615.3846153846152</v>
+      </c>
+      <c r="AO29">
+        <v>1084</v>
+      </c>
+      <c r="AP29">
+        <f t="shared" si="18"/>
+        <v>1.0840000000000001</v>
+      </c>
+      <c r="AQ29">
+        <f t="shared" si="19"/>
+        <v>4612.5461254612546</v>
+      </c>
+    </row>
+    <row r="30" spans="5:43">
       <c r="E30">
         <v>107</v>
       </c>
@@ -5405,8 +6595,52 @@
         <f t="shared" si="11"/>
         <v>4658.3850931677016</v>
       </c>
-    </row>
-    <row r="31" spans="5:27">
+      <c r="AC30">
+        <v>768</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="12"/>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="13"/>
+        <v>4557.291666666667</v>
+      </c>
+      <c r="AG30">
+        <v>869</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="14"/>
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="AI30">
+        <f t="shared" si="15"/>
+        <v>4602.9919447640968</v>
+      </c>
+      <c r="AK30">
+        <v>982</v>
+      </c>
+      <c r="AL30">
+        <f t="shared" si="16"/>
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="AM30">
+        <f t="shared" si="17"/>
+        <v>4582.4847250509165</v>
+      </c>
+      <c r="AO30">
+        <v>1088</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" si="18"/>
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="AQ30">
+        <f t="shared" si="19"/>
+        <v>4595.5882352941171</v>
+      </c>
+    </row>
+    <row r="31" spans="5:43">
       <c r="E31">
         <v>111</v>
       </c>
@@ -5473,8 +6707,52 @@
         <f t="shared" si="11"/>
         <v>4538.5779122541599</v>
       </c>
-    </row>
-    <row r="32" spans="5:27">
+      <c r="AC31">
+        <v>752</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="12"/>
+        <v>0.752</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="13"/>
+        <v>4654.255319148936</v>
+      </c>
+      <c r="AG31">
+        <v>862</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="14"/>
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="AI31">
+        <f t="shared" si="15"/>
+        <v>4640.3712296983758</v>
+      </c>
+      <c r="AK31">
+        <v>984</v>
+      </c>
+      <c r="AL31">
+        <f t="shared" si="16"/>
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="17"/>
+        <v>4573.1707317073169</v>
+      </c>
+      <c r="AO31">
+        <v>1084</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="18"/>
+        <v>1.0840000000000001</v>
+      </c>
+      <c r="AQ31">
+        <f t="shared" si="19"/>
+        <v>4612.5461254612546</v>
+      </c>
+    </row>
+    <row r="32" spans="5:43">
       <c r="E32">
         <v>112</v>
       </c>
@@ -5541,8 +6819,52 @@
         <f t="shared" si="11"/>
         <v>4587.1559633027518</v>
       </c>
-    </row>
-    <row r="33" spans="3:27">
+      <c r="AC32">
+        <v>744</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="12"/>
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="13"/>
+        <v>4704.3010752688169</v>
+      </c>
+      <c r="AG32">
+        <v>867</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="14"/>
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="15"/>
+        <v>4613.6101499423303</v>
+      </c>
+      <c r="AK32">
+        <v>978</v>
+      </c>
+      <c r="AL32">
+        <f t="shared" si="16"/>
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="AM32">
+        <f t="shared" si="17"/>
+        <v>4601.2269938650306</v>
+      </c>
+      <c r="AO32">
+        <v>1077</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="18"/>
+        <v>1.077</v>
+      </c>
+      <c r="AQ32">
+        <f t="shared" si="19"/>
+        <v>4642.5255338904362</v>
+      </c>
+    </row>
+    <row r="33" spans="3:43">
       <c r="E33">
         <v>115</v>
       </c>
@@ -5609,8 +6931,52 @@
         <f t="shared" si="11"/>
         <v>4622.4961479198764</v>
       </c>
-    </row>
-    <row r="35" spans="3:27">
+      <c r="AC33">
+        <v>748</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="12"/>
+        <v>0.748</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" si="13"/>
+        <v>4679.1443850267378</v>
+      </c>
+      <c r="AG33">
+        <v>852</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="14"/>
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="AI33">
+        <f t="shared" si="15"/>
+        <v>4694.8356807511736</v>
+      </c>
+      <c r="AK33">
+        <v>969</v>
+      </c>
+      <c r="AL33">
+        <f t="shared" si="16"/>
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="AM33">
+        <f t="shared" si="17"/>
+        <v>4643.9628482972139</v>
+      </c>
+      <c r="AO33">
+        <v>1076</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="18"/>
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="AQ33">
+        <f t="shared" si="19"/>
+        <v>4646.8401486988841</v>
+      </c>
+    </row>
+    <row r="35" spans="3:43">
       <c r="D35" t="s">
         <v>11</v>
       </c>
@@ -5638,8 +7004,24 @@
         <f>AVERAGE(AA4:AA33)</f>
         <v>4598.0262981304313</v>
       </c>
-    </row>
-    <row r="36" spans="3:27">
+      <c r="AE35">
+        <f>AVERAGE(AE4:AE33)</f>
+        <v>4612.4383927820099</v>
+      </c>
+      <c r="AI35">
+        <f>AVERAGE(AI4:AI33)</f>
+        <v>4631.8522736749983</v>
+      </c>
+      <c r="AM35">
+        <f>AVERAGE(AM4:AM33)</f>
+        <v>4582.4437623938438</v>
+      </c>
+      <c r="AQ35">
+        <f>AVERAGE(AQ4:AQ33)</f>
+        <v>4579.5222139732123</v>
+      </c>
+    </row>
+    <row r="36" spans="3:43">
       <c r="D36" t="s">
         <v>12</v>
       </c>
@@ -5667,23 +7049,39 @@
         <f>STDEV(AA4:AA33)</f>
         <v>51.520099144704375</v>
       </c>
-    </row>
-    <row r="40" spans="3:27">
+      <c r="AE36">
+        <f>STDEV(AE4:AE33)</f>
+        <v>108.00818827142608</v>
+      </c>
+      <c r="AI36">
+        <f>STDEV(AI4:AI33)</f>
+        <v>35.082988353644666</v>
+      </c>
+      <c r="AM36">
+        <f>STDEV(AM4:AM33)</f>
+        <v>78.29474052081693</v>
+      </c>
+      <c r="AQ36">
+        <f>STDEV(AQ4:AQ33)</f>
+        <v>85.010695250585258</v>
+      </c>
+    </row>
+    <row r="40" spans="3:43">
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40">
-        <f>AVERAGE(G35,K35,O35,S35,W35,AA35)</f>
-        <v>4598.6843548631914</v>
-      </c>
-    </row>
-    <row r="41" spans="3:27">
+        <f>AVERAGE(G35,K35,O35,S35,W35,AA35,AE35,AI35,AM35,AQ35)</f>
+        <v>4599.836277200322</v>
+      </c>
+    </row>
+    <row r="41" spans="3:43">
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41">
-        <f>AVERAGE(G36,K36,O36,S36,W36,AA36)</f>
-        <v>73.183888854955597</v>
+        <f>AVERAGE(G36,K36,O36,S36,W36,AA36,AE36,AI36,AM36,AQ36)</f>
+        <v>74.549994552620646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RSA performance graphs added
</commit_message>
<xml_diff>
--- a/katatsubaVSgradeschool.xlsx
+++ b/katatsubaVSgradeschool.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="primenumber" sheetId="2" r:id="rId2"/>
     <sheet name="Random" sheetId="3" r:id="rId3"/>
+    <sheet name="rsa" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Digits</t>
   </si>
@@ -66,6 +67,21 @@
   </si>
   <si>
     <t>Num/sec</t>
+  </si>
+  <si>
+    <t>e/sec</t>
+  </si>
+  <si>
+    <t>r/sec</t>
+  </si>
+  <si>
+    <t>r/Sec</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>STDev</t>
   </si>
 </sst>
 </file>
@@ -114,8 +130,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -170,7 +202,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -196,6 +228,14 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -221,6 +261,14 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,11 +476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115728552"/>
-        <c:axId val="2115718040"/>
+        <c:axId val="-2136668136"/>
+        <c:axId val="-2136674984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115728552"/>
+        <c:axId val="-2136668136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -460,7 +508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115718040"/>
+        <c:crossAx val="-2136674984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -468,7 +516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115718040"/>
+        <c:axId val="-2136674984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115728552"/>
+        <c:crossAx val="-2136668136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -505,6 +553,160 @@
       <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Encryption &amp; Decryption Time</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>rsa!$B$27:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>rsa!$C$27:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>803.031952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>673.387028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>539.739759</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>461.6895297415731</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>569.0413317105211</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>432.3660556315724</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2137972744"/>
+        <c:axId val="-2136444264"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2137972744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2136444264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2136444264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2137972744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -531,6 +733,41 @@
       <xdr:colOff>787400</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3542,7 +3779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -7093,4 +7330,882 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Y32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:25">
+      <c r="C1">
+        <v>32</v>
+      </c>
+      <c r="G1">
+        <v>65</v>
+      </c>
+      <c r="K1">
+        <v>94</v>
+      </c>
+      <c r="O1">
+        <v>127</v>
+      </c>
+      <c r="S1">
+        <v>160</v>
+      </c>
+      <c r="W1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25">
+      <c r="C4">
+        <v>53122048</v>
+      </c>
+      <c r="D4">
+        <f>C4/1000000000</f>
+        <v>5.3122047999999998E-2</v>
+      </c>
+      <c r="E4">
+        <f>$C$1/D4</f>
+        <v>602.38641401777284</v>
+      </c>
+      <c r="G4">
+        <v>67617024</v>
+      </c>
+      <c r="H4">
+        <f>G4/1000000000</f>
+        <v>6.7617023999999998E-2</v>
+      </c>
+      <c r="I4">
+        <f>$G$1/H4</f>
+        <v>961.29637412022157</v>
+      </c>
+      <c r="K4">
+        <v>313559808</v>
+      </c>
+      <c r="L4">
+        <f>K4/1000000000</f>
+        <v>0.313559808</v>
+      </c>
+      <c r="M4">
+        <f>$K$1/L4</f>
+        <v>299.7833191682526</v>
+      </c>
+      <c r="O4">
+        <v>136888064</v>
+      </c>
+      <c r="P4">
+        <f>O4/1000000000</f>
+        <v>0.136888064</v>
+      </c>
+      <c r="Q4">
+        <f>$O$1/P4</f>
+        <v>927.76533094952674</v>
+      </c>
+      <c r="S4">
+        <v>88721152</v>
+      </c>
+      <c r="T4">
+        <f>S4/1000000000</f>
+        <v>8.8721151999999998E-2</v>
+      </c>
+      <c r="U4">
+        <f>$S$1/T4</f>
+        <v>1803.4030937740754</v>
+      </c>
+      <c r="W4">
+        <v>2167313920</v>
+      </c>
+      <c r="X4">
+        <f>W4/1000000000</f>
+        <v>2.1673139199999998</v>
+      </c>
+      <c r="Y4">
+        <f>$W$1/X4</f>
+        <v>147.64820040467421</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25">
+      <c r="C5">
+        <v>266250752</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D13" si="0">C5/1000000000</f>
+        <v>0.26625075199999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E13" si="1">$C$1/D5</f>
+        <v>120.18745396820513</v>
+      </c>
+      <c r="G5">
+        <v>88499200</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H12" si="2">G5/1000000000</f>
+        <v>8.84992E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I13" si="3">$G$1/H5</f>
+        <v>734.46991611223609</v>
+      </c>
+      <c r="K5">
+        <v>134781184</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L13" si="4">K5/1000000000</f>
+        <v>0.134781184</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M13" si="5">$K$1/L5</f>
+        <v>697.42672686418905</v>
+      </c>
+      <c r="O5">
+        <v>911124992</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P13" si="6">O5/1000000000</f>
+        <v>0.91112499199999997</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q13" si="7">$O$1/P5</f>
+        <v>139.38812030742758</v>
+      </c>
+      <c r="S5">
+        <v>214459136</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T13" si="8">S5/1000000000</f>
+        <v>0.21445913599999999</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U13" si="9">$S$1/T5</f>
+        <v>746.06287698557173</v>
+      </c>
+      <c r="W5">
+        <v>1436342016</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ref="X5:X13" si="10">W5/1000000000</f>
+        <v>1.436342016</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ref="Y5:Y13" si="11">$W$1/X5</f>
+        <v>222.78816356786155</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25">
+      <c r="C6">
+        <v>38042112</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3.8042112000000003E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>841.17306631135511</v>
+      </c>
+      <c r="G6">
+        <v>61540096</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>6.1540096000000002E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>1056.2219467450943</v>
+      </c>
+      <c r="K6">
+        <v>171378176</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>0.17137817599999999</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>548.49457611218827</v>
+      </c>
+      <c r="O6">
+        <v>542213120</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>0.54221311999999999</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="7"/>
+        <v>234.22524338769227</v>
+      </c>
+      <c r="S6">
+        <v>657909760</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="8"/>
+        <v>0.65790976000000001</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="9"/>
+        <v>243.19444660617285</v>
+      </c>
+      <c r="W6">
+        <v>367847936</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="10"/>
+        <v>0.36784793599999999</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="11"/>
+        <v>869.92468540043683</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25">
+      <c r="C7">
+        <v>19833856</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.9833856E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1613.4028602405906</v>
+      </c>
+      <c r="G7">
+        <v>413701120</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.41370111999999998</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>157.11825967500403</v>
+      </c>
+      <c r="K7">
+        <v>135877120</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>0.13587711999999999</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>691.80153362096587</v>
+      </c>
+      <c r="O7">
+        <v>819853824</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>0.81985382399999995</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="7"/>
+        <v>154.90566279288345</v>
+      </c>
+      <c r="S7">
+        <v>262841088</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="8"/>
+        <v>0.262841088</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="9"/>
+        <v>608.73283251665737</v>
+      </c>
+      <c r="W7">
+        <v>544769024</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="10"/>
+        <v>0.54476902400000005</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="11"/>
+        <v>587.40491089302463</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25">
+      <c r="C8">
+        <v>121968896</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.12196889599999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>262.36197136686388</v>
+      </c>
+      <c r="G8">
+        <v>334111744</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.33411174399999999</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>194.54569067766741</v>
+      </c>
+      <c r="K8">
+        <v>159122944</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>0.15912294399999999</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>590.73819046485221</v>
+      </c>
+      <c r="O8">
+        <v>242187008</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>0.24218700800000001</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>524.38816206028685</v>
+      </c>
+      <c r="S8">
+        <v>325097984</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="8"/>
+        <v>0.32509798400000001</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="9"/>
+        <v>492.15931157542951</v>
+      </c>
+      <c r="W8">
+        <v>827433728</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="10"/>
+        <v>0.82743372800000003</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="11"/>
+        <v>386.7379213238936</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25">
+      <c r="C9">
+        <v>21594112</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.1594111999999999E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1481.8854324734448</v>
+      </c>
+      <c r="G9">
+        <v>33984000</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>3.3984E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>1912.6647834274952</v>
+      </c>
+      <c r="K9">
+        <v>338017280</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>0.33801727999999998</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>278.09229161302051</v>
+      </c>
+      <c r="O9">
+        <v>159045888</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>0.159045888</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>798.51168487927214</v>
+      </c>
+      <c r="S9">
+        <v>383066880</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="8"/>
+        <v>0.38306688</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="9"/>
+        <v>417.68163303494157</v>
+      </c>
+      <c r="W9">
+        <v>372804096</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="10"/>
+        <v>0.37280409599999997</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="11"/>
+        <v>858.35966780794172</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25">
+      <c r="C10">
+        <v>102479104</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.102479104</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>312.25878009237863</v>
+      </c>
+      <c r="G10">
+        <v>66209024</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>6.6209024000000005E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>981.73928677758477</v>
+      </c>
+      <c r="K10">
+        <v>513571072</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>0.51357107199999996</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>183.03211595220068</v>
+      </c>
+      <c r="O10">
+        <v>407855104</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>0.40785510400000002</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="7"/>
+        <v>311.38509425151142</v>
+      </c>
+      <c r="S10">
+        <v>310962176</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="8"/>
+        <v>0.31096217599999998</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="9"/>
+        <v>514.53203105962314</v>
+      </c>
+      <c r="W10">
+        <v>766306816</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="10"/>
+        <v>0.76630681599999995</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="11"/>
+        <v>417.58730748389951</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25">
+      <c r="C11">
+        <v>39680000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3.968E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>806.45161290322585</v>
+      </c>
+      <c r="G11">
+        <v>583544832</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.58354483199999996</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>111.38818550962679</v>
+      </c>
+      <c r="K11">
+        <v>113496064</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>0.11349606399999999</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>828.22255404381258</v>
+      </c>
+      <c r="O11">
+        <v>1996368384</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>1.9963683839999999</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="7"/>
+        <v>63.615513558443531</v>
+      </c>
+      <c r="S11">
+        <v>369553664</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="8"/>
+        <v>0.369553664</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="9"/>
+        <v>432.95471155171663</v>
+      </c>
+      <c r="W11">
+        <v>1313764096</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="10"/>
+        <v>1.3137640960000001</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="11"/>
+        <v>243.5749317356896</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25">
+      <c r="C12">
+        <v>43975680</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>4.3975680000000003E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>727.6749330539061</v>
+      </c>
+      <c r="G12">
+        <v>298854144</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0.29885414399999999</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>217.49740234487095</v>
+      </c>
+      <c r="K12">
+        <v>421916928</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>0.42191692800000002</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>222.7926725898042</v>
+      </c>
+      <c r="O12">
+        <v>104243200</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>0.10424319999999999</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="7"/>
+        <v>1218.3048870333989</v>
+      </c>
+      <c r="S12">
+        <v>1839032064</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="8"/>
+        <v>1.839032064</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="9"/>
+        <v>87.002289482648195</v>
+      </c>
+      <c r="W12">
+        <v>1111214080</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="10"/>
+        <v>1.1112140800000001</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="11"/>
+        <v>287.97331293714348</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25">
+      <c r="C13">
+        <v>25345792</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2.5345791999999999E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1262.5369923338753</v>
+      </c>
+      <c r="G13">
+        <v>159733248</v>
+      </c>
+      <c r="H13">
+        <f>G13/1000000000</f>
+        <v>0.15973324799999999</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>406.92843108029706</v>
+      </c>
+      <c r="K13">
+        <v>88929792</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>8.8929791999999994E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>1057.0136046196983</v>
+      </c>
+      <c r="O13">
+        <v>519628032</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>0.51962803199999996</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="7"/>
+        <v>244.40559819528752</v>
+      </c>
+      <c r="S13">
+        <v>464185088</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="8"/>
+        <v>0.46418508800000002</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="9"/>
+        <v>344.69009051837526</v>
+      </c>
+      <c r="W13">
+        <v>1060791808</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="10"/>
+        <v>1.0607918080000001</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="11"/>
+        <v>301.66145476115895</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(E4:E13)</f>
+        <v>803.03195167616173</v>
+      </c>
+      <c r="I15">
+        <f>AVERAGE(I4:I13)</f>
+        <v>673.38702764700986</v>
+      </c>
+      <c r="M15">
+        <f>AVERAGE(M4:M13)</f>
+        <v>539.73975850489853</v>
+      </c>
+      <c r="Q15">
+        <f>AVERAGE(Q4:Q13)</f>
+        <v>461.6895297415731</v>
+      </c>
+      <c r="U15">
+        <f>AVERAGE(U4:U13)</f>
+        <v>569.04133171052115</v>
+      </c>
+      <c r="Y15">
+        <f>AVERAGE(Y4:Y13)</f>
+        <v>432.36605563157235</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <f>STDEV(E4:E13)</f>
+        <v>513.76071306250549</v>
+      </c>
+      <c r="I16">
+        <f>STDEV(I4:I13)</f>
+        <v>572.96273463212208</v>
+      </c>
+      <c r="M16">
+        <f>STDEV(M4:M13)</f>
+        <v>289.67305186048003</v>
+      </c>
+      <c r="Q16">
+        <f>STDEV(Q4:Q13)</f>
+        <v>392.29735430520702</v>
+      </c>
+      <c r="U16">
+        <f>STDEV(U4:U13)</f>
+        <v>470.9026495298379</v>
+      </c>
+      <c r="Y16">
+        <f>STDEV(Y4:Y13)</f>
+        <v>257.73105965511326</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <f>AVERAGE(E15,I15,M15,Q15,U15,Y15)</f>
+        <v>579.87594248528944</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f>AVERAGE(E16,I16,M16,Q16,U16,Y16)</f>
+        <v>416.22126050754429</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>803.03195200000005</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28">
+        <v>65</v>
+      </c>
+      <c r="C28">
+        <v>673.38702799999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29">
+        <v>94</v>
+      </c>
+      <c r="C29">
+        <v>539.73975900000005</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30">
+        <v>127</v>
+      </c>
+      <c r="C30">
+        <f>AVERAGE(Q4:Q13)</f>
+        <v>461.6895297415731</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31">
+        <v>160</v>
+      </c>
+      <c r="C31">
+        <f>AVERAGE(U4:U13)</f>
+        <v>569.04133171052115</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32">
+        <v>320</v>
+      </c>
+      <c r="C32">
+        <f>AVERAGE(Y4:Y13)</f>
+        <v>432.36605563157235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
something added which I do not remember
</commit_message>
<xml_diff>
--- a/katatsubaVSgradeschool.xlsx
+++ b/katatsubaVSgradeschool.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="10720" yWindow="340" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="primenumber" sheetId="2" r:id="rId2"/>
     <sheet name="Random" sheetId="3" r:id="rId3"/>
     <sheet name="rsa" sheetId="4" r:id="rId4"/>
+    <sheet name="performance" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Digits</t>
   </si>
@@ -83,12 +84,24 @@
   <si>
     <t>STDev</t>
   </si>
+  <si>
+    <t>OUR</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>bits</t>
+  </si>
+  <si>
+    <t>Their</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +125,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +151,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -198,11 +219,85 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -236,6 +331,40 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -269,6 +398,40 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,11 +639,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2136668136"/>
-        <c:axId val="-2136674984"/>
+        <c:axId val="-2137603448"/>
+        <c:axId val="-2137596616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2136668136"/>
+        <c:axId val="-2137603448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136674984"/>
+        <c:crossAx val="-2137596616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -516,7 +679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136674984"/>
+        <c:axId val="-2137596616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136668136"/>
+        <c:crossAx val="-2137603448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -664,11 +827,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137972744"/>
-        <c:axId val="-2136444264"/>
+        <c:axId val="-2136543000"/>
+        <c:axId val="-2136539992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137972744"/>
+        <c:axId val="-2136543000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136444264"/>
+        <c:crossAx val="-2136539992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -686,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136444264"/>
+        <c:axId val="-2136539992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +859,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137972744"/>
+        <c:crossAx val="-2136543000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7336,7 +7499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27:C32"/>
     </sheetView>
   </sheetViews>
@@ -8208,4 +8371,146 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" s="2" customFormat="1">
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="1">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1">
+        <v>78310144</v>
+      </c>
+      <c r="D4" s="1">
+        <v>27386368</v>
+      </c>
+      <c r="F4" s="1">
+        <f>C4/1000000</f>
+        <v>78.310143999999994</v>
+      </c>
+      <c r="G4" s="1">
+        <f>D4/1000000</f>
+        <v>27.386368000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="1">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1">
+        <v>33817088</v>
+      </c>
+      <c r="D5" s="1">
+        <v>320994816</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F8" si="0">C5/1000000</f>
+        <v>33.817087999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G8" si="1">D5/1000000</f>
+        <v>320.99481600000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="1">
+        <v>160</v>
+      </c>
+      <c r="C6" s="1">
+        <v>160193792</v>
+      </c>
+      <c r="D6" s="1">
+        <v>963482880</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>160.193792</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>963.48288000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="1">
+        <v>220</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2901262848</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10155141120</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>2901.2628479999998</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>10155.14112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="1">
+        <v>273</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4219404032</v>
+      </c>
+      <c r="D8" s="1">
+        <v>33831159296</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>4219.4040320000004</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>33831.159295999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>